<commit_message>
for now, download excel reg students remain
</commit_message>
<xml_diff>
--- a/controllers/2.xlsx
+++ b/controllers/2.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <definedNames/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Roll No</t>
   </si>
@@ -22,7 +23,7 @@
     <t>Email ID</t>
   </si>
   <si>
-    <t>student1@example.com</t>
+    <t>aswanibolisetti@gmail.com</t>
   </si>
   <si>
     <t>student2@example.com</t>
@@ -35,19 +36,28 @@
   </si>
   <si>
     <t>student5@example.com</t>
+  </si>
+  <si>
+    <t>student@example.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -87,23 +97,124 @@
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
-      <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="20">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="15" builtinId="5"/>
+    <cellStyle name="Currency" xfId="16" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="17" builtinId="7"/>
+    <cellStyle name="Comma" xfId="18" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="19" builtinId="6"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -391,14 +502,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1">
+      <selection pane="topLeft" activeCell="B8" sqref="B8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" ht="15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -406,7 +519,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" ht="15">
       <c r="A2">
         <v>1</v>
       </c>
@@ -414,7 +527,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" ht="15">
       <c r="A3">
         <v>2</v>
       </c>
@@ -422,7 +535,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" ht="15">
       <c r="A4">
         <v>3</v>
       </c>
@@ -430,7 +543,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" ht="15">
       <c r="A5">
         <v>4</v>
       </c>
@@ -438,12 +551,25 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" ht="15">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="15">
+      <c r="A8">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>